<commit_message>
Added 'AutoSPInstaller ' Build 3.96 with SP2013 Service Pack 1 support
</commit_message>
<xml_diff>
--- a/SharePoint/AutoSPInstaller/AutoSPInstaller_Usage_Notes.xlsx
+++ b/SharePoint/AutoSPInstaller/AutoSPInstaller_Usage_Notes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Configuration Section</t>
   </si>
@@ -49,6 +49,30 @@
   </si>
   <si>
     <t>&lt;AutoAdminLogon Enable="true" Password="DevPassword123"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;ManagedAccounts&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ManagedAccount CommonName="spservice"&gt;
+                &lt;Username&gt;DOMAIN\SP_Services&lt;/Username&gt;
+                &lt;Password&gt;&lt;/Password&gt;
+            &lt;/ManagedAccount&gt;
+            &lt;ManagedAccount CommonName="Portal"&gt;
+                &lt;Username&gt;DOMAIN\SP_PortalAppPool&lt;/Username&gt;
+                &lt;Password&gt;&lt;/Password&gt;
+            &lt;/ManagedAccount&gt;
+            &lt;ManagedAccount CommonName="MySiteHost"&gt;
+                &lt;Username&gt;DOMAIN\SP_ProfilesAppPool&lt;/Username&gt;
+                &lt;Password&gt;&lt;/Password&gt;
+            &lt;/ManagedAccount&gt;
+            &lt;ManagedAccount CommonName="SearchService"&gt;
+                &lt;Username&gt;DOMAIN\SP_SearchService&lt;/Username&gt;
+                &lt;Password&gt;&lt;/Password&gt;
+            &lt;/ManagedAccount&gt;</t>
+  </si>
+  <si>
+    <t>When provisioning Managed Accounts it is important to leave the 'CommonName' property set to what they are for the 4 default accounts. This property is now bound to the default 'Portal' and 'My Site' web applications; and the Search Service Applications - so should be left in place.</t>
   </si>
 </sst>
 </file>
@@ -399,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,6 +479,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3.96</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>